<commit_message>
Trying to add compostion to the terms.
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Atoms" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
   <si>
     <t>[Concept]</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>I[B];t</t>
+  </si>
+  <si>
+    <t>Composition</t>
+  </si>
+  <si>
+    <t>[Composition]</t>
   </si>
 </sst>
 </file>
@@ -652,7 +658,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -698,90 +704,96 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
       </c>
       <c r="E2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>32</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -789,138 +801,141 @@
         <v>33</v>
       </c>
       <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>35</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>36</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>37</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>34</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>34</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>36</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>36</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>34</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>24</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>38</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>24</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>34</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>25</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Braga.xlsx does not import ...  (for Han)
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Terms" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -656,18 +657,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
+    <row r="1" spans="1:5">
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -675,7 +673,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -686,7 +684,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -695,6 +693,11 @@
       </c>
       <c r="C3" s="1" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="E6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP + specify binding by hand
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>[Concept]</t>
   </si>
@@ -122,24 +122,6 @@
     <t>;</t>
   </si>
   <si>
-    <t>I[A];r;I[C]</t>
-  </si>
-  <si>
-    <t>I[A];r</t>
-  </si>
-  <si>
-    <t>I[A];s;I[B]</t>
-  </si>
-  <si>
-    <t>I[A];s</t>
-  </si>
-  <si>
-    <t>I[B];t;I[C]</t>
-  </si>
-  <si>
-    <t>I[B];t</t>
-  </si>
-  <si>
     <t>t1</t>
   </si>
   <si>
@@ -164,15 +146,6 @@
     <t>t8</t>
   </si>
   <si>
-    <t>t9</t>
-  </si>
-  <si>
-    <t>t10</t>
-  </si>
-  <si>
-    <t>t11</t>
-  </si>
-  <si>
     <t>r1</t>
   </si>
   <si>
@@ -195,6 +168,18 @@
   </si>
   <si>
     <t>Intersection</t>
+  </si>
+  <si>
+    <t>r[A*C]</t>
+  </si>
+  <si>
+    <t>s[A*B]</t>
+  </si>
+  <si>
+    <t>t[B*C]</t>
+  </si>
+  <si>
+    <t>bind</t>
   </si>
 </sst>
 </file>
@@ -568,7 +553,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -664,7 +649,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -678,7 +663,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -692,7 +677,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -740,13 +725,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -761,139 +746,130 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
         <v>26</v>
       </c>
     </row>
@@ -904,17 +880,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A8" sqref="A8:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
@@ -928,7 +904,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -942,114 +918,30 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B7" t="s">
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1059,57 +951,27 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A15"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="A8" sqref="A8:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1129,17 +991,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Rule to computation of pretypes
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -16,12 +16,12 @@
     <sheet name="Compositions" sheetId="8" r:id="rId7"/>
     <sheet name="Intersections" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
   <si>
     <t>[Concept]</t>
   </si>
@@ -113,9 +113,6 @@
     <t>target</t>
   </si>
   <si>
-    <t>r/\s;t</t>
-  </si>
-  <si>
     <t>s;t</t>
   </si>
   <si>
@@ -180,6 +177,15 @@
   </si>
   <si>
     <t>bind</t>
+  </si>
+  <si>
+    <t>r ISC s;t</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>s;t = r ISC s;t</t>
   </si>
 </sst>
 </file>
@@ -215,9 +221,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -614,7 +621,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +656,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -658,12 +665,12 @@
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -672,12 +679,12 @@
         <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -696,15 +703,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
       <c r="B1" t="s">
         <v>19</v>
       </c>
@@ -712,7 +722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -723,20 +733,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>17</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -749,7 +754,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,7 +767,7 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,75 +783,83 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -880,17 +893,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD15"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
@@ -904,7 +917,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
@@ -918,29 +931,43 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
         <v>36</v>
-      </c>
-      <c r="B6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
         <v>34</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -961,17 +988,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -991,17 +1018,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
remove Rule ISA Term from domain analysis
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Atoms" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>[Concept]</t>
   </si>
@@ -95,15 +95,6 @@
     <t>operator</t>
   </si>
   <si>
-    <t>I[A]</t>
-  </si>
-  <si>
-    <t>I[B]</t>
-  </si>
-  <si>
-    <t>I[C]</t>
-  </si>
-  <si>
     <t>Operator</t>
   </si>
   <si>
@@ -170,9 +161,6 @@
     <t>r[A*C]</t>
   </si>
   <si>
-    <t>s[A*B]</t>
-  </si>
-  <si>
     <t>t[B*C]</t>
   </si>
   <si>
@@ -182,10 +170,22 @@
     <t>r ISC s;t</t>
   </si>
   <si>
-    <t>=</t>
-  </si>
-  <si>
     <t>s;t = r ISC s;t</t>
+  </si>
+  <si>
+    <t>r = s;t</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>s[B*A]</t>
+  </si>
+  <si>
+    <t>leftTerm</t>
+  </si>
+  <si>
+    <t>riteTerm</t>
   </si>
 </sst>
 </file>
@@ -221,10 +221,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -560,7 +558,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,7 +619,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,10 +632,10 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -656,7 +654,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -670,21 +668,21 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -703,45 +701,173 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -749,161 +875,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>41</v>
       </c>
       <c r="B1" t="s">
         <v>23</v>
@@ -915,12 +899,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -929,46 +913,32 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -988,17 +958,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1008,27 +978,27 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
generate TypeTerm for Composition in domain analysis
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Atoms" sheetId="2" r:id="rId1"/>
@@ -179,13 +179,13 @@
     <t>r2</t>
   </si>
   <si>
-    <t>s[B*A]</t>
-  </si>
-  <si>
     <t>leftTerm</t>
   </si>
   <si>
     <t>riteTerm</t>
+  </si>
+  <si>
+    <t>s[A*B]</t>
   </si>
 </sst>
 </file>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,10 +674,10 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -703,7 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -717,10 +717,10 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
         <v>53</v>
-      </c>
-      <c r="D1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -770,7 +770,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -859,7 +859,7 @@
         <v>35</v>
       </c>
       <c r="B10" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
All rules from the paper [RAMiCS 2015] are included in DomainAnalysis.adl
@sjcjoosten, please review DomainAnalysis.adl. To run the program, compile Terms.ifc and encode your script in Braga.xlsx
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Atoms" sheetId="2" r:id="rId1"/>
@@ -185,7 +185,7 @@
     <t>riteTerm</t>
   </si>
   <si>
-    <t>s[A*B]</t>
+    <t>s[B*A]</t>
   </si>
 </sst>
 </file>
@@ -618,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -674,10 +674,10 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -769,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
try new {EX} regime for _; delimite
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Atoms" sheetId="2" r:id="rId1"/>
@@ -16,12 +16,12 @@
     <sheet name="Compositions" sheetId="8" r:id="rId7"/>
     <sheet name="Intersections" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
   <si>
     <t>[Concept]</t>
   </si>
@@ -186,13 +186,22 @@
   </si>
   <si>
     <t>s[B*A]</t>
+  </si>
+  <si>
+    <t>Context</t>
+  </si>
+  <si>
+    <t>Braga</t>
+  </si>
+  <si>
+    <t>context</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,7 +247,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -312,7 +321,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -347,7 +355,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -523,16 +530,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -540,7 +547,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -554,16 +561,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +581,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -585,7 +592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -593,7 +600,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -601,7 +608,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -615,16 +622,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -638,7 +645,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -652,7 +659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -666,7 +673,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -680,7 +687,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -700,16 +707,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -723,7 +730,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -737,7 +744,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -751,7 +758,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="F6" t="s">
         <v>37</v>
       </c>
@@ -766,107 +773,134 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>22</v>
       </c>
       <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>21</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>31</v>
       </c>
       <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
+    <row r="6" spans="1:6">
+      <c r="E6" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>34</v>
       </c>
       <c r="B9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>35</v>
       </c>
       <c r="B10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>36</v>
       </c>
       <c r="B11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s">
         <v>46</v>
       </c>
     </row>
@@ -876,16 +910,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>38</v>
       </c>
@@ -899,7 +933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>39</v>
       </c>
@@ -913,7 +947,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="F6" t="s">
         <v>32</v>
       </c>
@@ -927,7 +961,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -947,26 +981,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -977,26 +1011,26 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="C6" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
WIP: trying to make rules editable in the application
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Atoms" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
   <si>
     <t>[Concept]</t>
   </si>
@@ -194,7 +194,10 @@
     <t>Braga</t>
   </si>
   <si>
-    <t>context</t>
+    <t>rules~</t>
+  </si>
+  <si>
+    <t>relations~</t>
   </si>
 </sst>
 </file>
@@ -623,81 +626,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>34</v>
       </c>
       <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>35</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>36</v>
       </c>
       <c r="B5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -708,61 +726,70 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>51</v>
       </c>
       <c r="B3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="F6" t="s">
+    <row r="6" spans="1:8">
+      <c r="G6" t="s">
         <v>37</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>49</v>
       </c>
     </row>
@@ -776,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -786,9 +813,6 @@
       <c r="A1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
-        <v>57</v>
-      </c>
       <c r="C1" t="s">
         <v>6</v>
       </c>
@@ -800,9 +824,6 @@
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" t="s">
-        <v>55</v>
-      </c>
       <c r="C2" t="s">
         <v>11</v>
       </c>
@@ -814,9 +835,6 @@
       <c r="A3" t="s">
         <v>29</v>
       </c>
-      <c r="B3" t="s">
-        <v>56</v>
-      </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
@@ -828,9 +846,6 @@
       <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
       <c r="C4" t="s">
         <v>15</v>
       </c>
@@ -842,9 +857,6 @@
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
       <c r="C5" t="s">
         <v>16</v>
       </c>
@@ -864,9 +876,6 @@
       <c r="A7" t="s">
         <v>33</v>
       </c>
-      <c r="B7" t="s">
-        <v>56</v>
-      </c>
       <c r="C7" t="s">
         <v>27</v>
       </c>
@@ -875,9 +884,6 @@
       <c r="A9" t="s">
         <v>34</v>
       </c>
-      <c r="B9" t="s">
-        <v>56</v>
-      </c>
       <c r="C9" t="s">
         <v>45</v>
       </c>
@@ -886,9 +892,6 @@
       <c r="A10" t="s">
         <v>35</v>
       </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
       <c r="C10" t="s">
         <v>54</v>
       </c>
@@ -896,9 +899,6 @@
     <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
       </c>
       <c r="C11" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Braga-demo is now concentrated in one file.
The idea of this demo is to demonstrate the type system by gradually introducing more rules.
In practice, this is done by removing comments one-by-one.
</commit_message>
<xml_diff>
--- a/AmpersandData/FormalAmpersand/Braga.xlsx
+++ b/AmpersandData/FormalAmpersand/Braga.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="168" windowWidth="14808" windowHeight="7956" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Atoms" sheetId="2" r:id="rId1"/>
@@ -12,16 +12,15 @@
     <sheet name="Relations" sheetId="3" r:id="rId3"/>
     <sheet name="Rules" sheetId="4" r:id="rId4"/>
     <sheet name="Terms" sheetId="5" r:id="rId5"/>
-    <sheet name="Binary Terms" sheetId="7" r:id="rId6"/>
-    <sheet name="Compositions" sheetId="8" r:id="rId7"/>
-    <sheet name="Intersections" sheetId="9" r:id="rId8"/>
+    <sheet name="Compositions" sheetId="8" r:id="rId6"/>
+    <sheet name="Intersections" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="42">
   <si>
     <t>[Concept]</t>
   </si>
@@ -92,12 +91,6 @@
     <t>[Term]</t>
   </si>
   <si>
-    <t>operator</t>
-  </si>
-  <si>
-    <t>Operator</t>
-  </si>
-  <si>
     <t>source</t>
   </si>
   <si>
@@ -107,9 +100,6 @@
     <t>s;t</t>
   </si>
   <si>
-    <t>;</t>
-  </si>
-  <si>
     <t>t1</t>
   </si>
   <si>
@@ -125,27 +115,9 @@
     <t>t5</t>
   </si>
   <si>
-    <t>t6</t>
-  </si>
-  <si>
-    <t>t7</t>
-  </si>
-  <si>
-    <t>t8</t>
-  </si>
-  <si>
     <t>r1</t>
   </si>
   <si>
-    <t>[BinaryTerm]</t>
-  </si>
-  <si>
-    <t>BinaryTerm</t>
-  </si>
-  <si>
-    <t>/\</t>
-  </si>
-  <si>
     <t>[Composition]</t>
   </si>
   <si>
@@ -158,15 +130,6 @@
     <t>Intersection</t>
   </si>
   <si>
-    <t>r[A*C]</t>
-  </si>
-  <si>
-    <t>t[B*C]</t>
-  </si>
-  <si>
-    <t>bind</t>
-  </si>
-  <si>
     <t>r ISC s;t</t>
   </si>
   <si>
@@ -182,29 +145,14 @@
     <t>leftTerm</t>
   </si>
   <si>
-    <t>riteTerm</t>
-  </si>
-  <si>
-    <t>s[B*A]</t>
-  </si>
-  <si>
-    <t>Context</t>
-  </si>
-  <si>
-    <t>Braga</t>
-  </si>
-  <si>
-    <t>rules~</t>
-  </si>
-  <si>
-    <t>relations~</t>
+    <t>rightTerm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -250,7 +198,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Kantoor">
       <a:dk1>
@@ -324,6 +272,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -358,6 +307,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kantoor">
@@ -533,16 +483,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -550,7 +500,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -564,16 +514,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -595,7 +545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -603,7 +553,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -611,7 +561,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -625,97 +575,82 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -725,72 +660,63 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>52</v>
-      </c>
-      <c r="E1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
       <c r="G6" t="s">
         <v>37</v>
-      </c>
-      <c r="H6" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -800,108 +726,69 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A9" sqref="A9:XFD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="D6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>30</v>
       </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>46</v>
+      <c r="B7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -910,69 +797,49 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" t="s">
-        <v>40</v>
-      </c>
-      <c r="H6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -981,58 +848,46 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="C6" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>